<commit_message>
Update prescription-Intro.md with implementation guide notice
Added a warning about ongoing discussions for hosting the implementation guide on the ANS side and provided a link to the latest version of the ePrescription section. 47c2352e90ec23362441f3ee7cdc1c5c538f104a
</commit_message>
<xml_diff>
--- a/nriss-patch-1/ig/CodeSystem-fr-document-type.xlsx
+++ b/nriss-patch-1/ig/CodeSystem-fr-document-type.xlsx
@@ -25,7 +25,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://hl7.fr/fhir/fr/medication/CodeSystem/fr-document-type</t>
+    <t>https://hl7.fr/ig/fhir/medication/CodeSystem/fr-document-type</t>
   </si>
   <si>
     <t>Version</t>
@@ -61,7 +61,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-10T15:35:36+00:00</t>
+    <t>2026-01-15T08:54:26+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -79,7 +79,7 @@
     <t>Jurisdiction</t>
   </si>
   <si>
-    <t/>
+    <t>FRANCE</t>
   </si>
   <si>
     <t>Description</t>

</xml_diff>